<commit_message>
lecture 9 and 10 finger exercises
</commit_message>
<xml_diff>
--- a/time logging.xlsx
+++ b/time logging.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffen\Arbejde\CS education\Introduction To CS and Programming Using Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDB6107-3D3B-4DA6-890E-609943DA96A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B46E117-E3C7-4EBE-BE0E-75488CD2A9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-1980" windowWidth="16440" windowHeight="28440" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>CS Introduction lecture 7</t>
+  </si>
+  <si>
+    <t>CS Introduction lecture 8</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>CS Introduction lecture 9</t>
   </si>
 </sst>
 </file>
@@ -104,10 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -443,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE79405-D1A3-4A66-A83E-48D5F1755AB2}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -562,12 +570,58 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>45809</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F8" s="2"/>
-      <c r="G8" s="3"/>
+      <c r="A8" s="1">
+        <v>45810</v>
+      </c>
+      <c r="B8">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>21</v>
+      </c>
+      <c r="E8">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finger exercise lecture 11
</commit_message>
<xml_diff>
--- a/time logging.xlsx
+++ b/time logging.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffen\Arbejde\CS education\Introduction To CS and Programming Using Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE1DD60-7964-4691-900B-4630D189D4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122321AF-9977-4DD1-A4F9-FF959D020A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Problem Set 1</t>
+  </si>
+  <si>
+    <t>CS introduction lecture11</t>
+  </si>
+  <si>
+    <t>Problem Set 2</t>
   </si>
 </sst>
 </file>
@@ -457,7 +463,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,6 +640,40 @@
         <v>12</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>45811</v>
+      </c>
+      <c r="B10">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>19</v>
+      </c>
+      <c r="E10">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>45811</v>
+      </c>
+      <c r="B11">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="35" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E35" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
lecture 12 finger exercise
</commit_message>
<xml_diff>
--- a/time logging.xlsx
+++ b/time logging.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffen\Arbejde\CS education\Introduction To CS and Programming Using Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122321AF-9977-4DD1-A4F9-FF959D020A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36457BFB-4FFB-40E0-9211-10C4321572B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
+    <workbookView xWindow="38280" yWindow="-1980" windowWidth="16440" windowHeight="28440" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -68,9 +68,6 @@
     <t>CS Introduction lecture 8</t>
   </si>
   <si>
-    <t>asd</t>
-  </si>
-  <si>
     <t>CS Introduction lecture 9</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>Problem Set 2</t>
+  </si>
+  <si>
+    <t>CS introduction Lecture 12</t>
   </si>
 </sst>
 </file>
@@ -460,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE79405-D1A3-4A66-A83E-48D5F1755AB2}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -616,7 +616,7 @@
         <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -637,7 +637,7 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -657,7 +657,7 @@
         <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -665,21 +665,33 @@
         <v>45811</v>
       </c>
       <c r="B11">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11">
-        <v>37</v>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>21</v>
+      </c>
+      <c r="E11">
+        <v>40</v>
       </c>
       <c r="F11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>45812</v>
+      </c>
+      <c r="B12">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish finger exercises lecture 12
</commit_message>
<xml_diff>
--- a/time logging.xlsx
+++ b/time logging.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffen\Arbejde\CS education\Introduction To CS and Programming Using Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36457BFB-4FFB-40E0-9211-10C4321572B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A573D0C6-A3BA-4DD5-8066-D78E9C229E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-1980" windowWidth="16440" windowHeight="28440" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>CS introduction Lecture 12</t>
+  </si>
+  <si>
+    <t>CS intoduction Lecture 12</t>
   </si>
 </sst>
 </file>
@@ -460,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE79405-D1A3-4A66-A83E-48D5F1755AB2}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -690,8 +693,34 @@
       <c r="C12">
         <v>10</v>
       </c>
+      <c r="D12">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>38</v>
+      </c>
       <c r="F12" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>45813</v>
+      </c>
+      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finger exercise lecture 13
</commit_message>
<xml_diff>
--- a/time logging.xlsx
+++ b/time logging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffen\Arbejde\CS education\Introduction To CS and Programming Using Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A573D0C6-A3BA-4DD5-8066-D78E9C229E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB6B76B-5469-4AED-9E7B-4B13D33ED146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>CS intoduction Lecture 12</t>
+  </si>
+  <si>
+    <t>CS intoduction Lecture 13</t>
+  </si>
+  <si>
+    <t>CS intoduction Lecture 14</t>
   </si>
 </sst>
 </file>
@@ -463,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE79405-D1A3-4A66-A83E-48D5F1755AB2}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -723,6 +729,40 @@
         <v>15</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>45813</v>
+      </c>
+      <c r="B14">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>45813</v>
+      </c>
+      <c r="B15">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finger exercise lecture 14
</commit_message>
<xml_diff>
--- a/time logging.xlsx
+++ b/time logging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffen\Arbejde\CS education\Introduction To CS and Programming Using Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB6B76B-5469-4AED-9E7B-4B13D33ED146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D8BBDE-0581-4C33-8D4A-BEF9B3987EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
   </bookViews>
@@ -759,6 +759,12 @@
       <c r="C15">
         <v>15</v>
       </c>
+      <c r="D15">
+        <v>18</v>
+      </c>
+      <c r="E15">
+        <v>13</v>
+      </c>
       <c r="F15" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
finger exercises Lecture 15
</commit_message>
<xml_diff>
--- a/time logging.xlsx
+++ b/time logging.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffen\Arbejde\CS education\Introduction To CS and Programming Using Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steff\Personal\CS Education\CS-ducation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D8BBDE-0581-4C33-8D4A-BEF9B3987EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEB4C3B-D87C-4699-9FA5-3A24C59FAF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -83,13 +72,16 @@
     <t>CS introduction Lecture 12</t>
   </si>
   <si>
-    <t>CS intoduction Lecture 12</t>
-  </si>
-  <si>
-    <t>CS intoduction Lecture 13</t>
-  </si>
-  <si>
-    <t>CS intoduction Lecture 14</t>
+    <t>CS Introduction Lecture 12</t>
+  </si>
+  <si>
+    <t>CS Introduction Lecture 13</t>
+  </si>
+  <si>
+    <t>CS Introduction Lecture 14</t>
+  </si>
+  <si>
+    <t>CS Introduction Lecture 15</t>
   </si>
 </sst>
 </file>
@@ -469,18 +461,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE79405-D1A3-4A66-A83E-48D5F1755AB2}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -508,7 +500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>45808</v>
       </c>
@@ -528,7 +520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>45808</v>
       </c>
@@ -548,7 +540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>45808</v>
       </c>
@@ -568,7 +560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>45809</v>
       </c>
@@ -588,7 +580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>45809</v>
       </c>
@@ -608,7 +600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>45810</v>
       </c>
@@ -629,7 +621,7 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>45810</v>
       </c>
@@ -649,7 +641,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>45811</v>
       </c>
@@ -669,7 +661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>45811</v>
       </c>
@@ -689,7 +681,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>45812</v>
       </c>
@@ -709,7 +701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>45813</v>
       </c>
@@ -729,7 +721,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>45813</v>
       </c>
@@ -749,7 +741,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>45813</v>
       </c>
@@ -767,6 +759,26 @@
       </c>
       <c r="F15" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="1">
+        <v>45814</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>45</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finger exercise lecture 16
</commit_message>
<xml_diff>
--- a/time logging.xlsx
+++ b/time logging.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steff\Personal\CS Education\Python Introduction course\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffen\Arbejde\CS education\Introduction To CS and Programming Using Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A914ED61-0A5A-473D-B6B3-B34398F2E730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62A7A43-F310-4569-B8F9-C36736AC322D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Problem Set 3</t>
+  </si>
+  <si>
+    <t>CS Introduction Lecture 16</t>
   </si>
 </sst>
 </file>
@@ -464,18 +467,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE79405-D1A3-4A66-A83E-48D5F1755AB2}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.06640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -503,7 +506,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45808</v>
       </c>
@@ -523,7 +526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>45808</v>
       </c>
@@ -543,7 +546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45808</v>
       </c>
@@ -563,7 +566,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45809</v>
       </c>
@@ -583,7 +586,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45809</v>
       </c>
@@ -603,7 +606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>45810</v>
       </c>
@@ -624,7 +627,7 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>45810</v>
       </c>
@@ -644,7 +647,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>45811</v>
       </c>
@@ -664,7 +667,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>45811</v>
       </c>
@@ -684,7 +687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>45812</v>
       </c>
@@ -704,7 +707,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>45813</v>
       </c>
@@ -724,7 +727,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>45813</v>
       </c>
@@ -744,7 +747,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>45813</v>
       </c>
@@ -764,7 +767,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>45814</v>
       </c>
@@ -784,7 +787,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>45815</v>
       </c>
@@ -804,7 +807,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>45816</v>
       </c>
@@ -824,7 +827,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>45817</v>
       </c>
@@ -842,6 +845,46 @@
       </c>
       <c r="F19" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>45818</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>50</v>
+      </c>
+      <c r="D20">
+        <v>21</v>
+      </c>
+      <c r="E20">
+        <v>46</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>45819</v>
+      </c>
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>19</v>
+      </c>
+      <c r="E21">
+        <v>50</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finger excercises lecture 18
</commit_message>
<xml_diff>
--- a/time logging.xlsx
+++ b/time logging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steff\Personal\CS Education\Python Introduction course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17762901-CD1C-4C31-911E-1870A84C56A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FEE2C8-0E8E-4952-85E1-4D3CC938FC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>CS Introduction Lecture 17</t>
+  </si>
+  <si>
+    <t>CS Introduction Lecture 18</t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -911,7 +914,24 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1">
+        <v>45822</v>
+      </c>
+      <c r="B23">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>41</v>
+      </c>
+      <c r="D23">
+        <v>12</v>
+      </c>
+      <c r="E23">
+        <v>17</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
finger exercises lecture 19
</commit_message>
<xml_diff>
--- a/time logging.xlsx
+++ b/time logging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steff\Personal\CS Education\Python Introduction course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FEE2C8-0E8E-4952-85E1-4D3CC938FC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E339ECF-777B-448F-81B0-FCE4D8735A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -473,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE79405-D1A3-4A66-A83E-48D5F1755AB2}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -933,6 +933,26 @@
         <v>22</v>
       </c>
     </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="1">
+        <v>45822</v>
+      </c>
+      <c r="B24">
+        <v>14</v>
+      </c>
+      <c r="C24">
+        <v>30</v>
+      </c>
+      <c r="D24">
+        <v>15</v>
+      </c>
+      <c r="E24">
+        <v>30</v>
+      </c>
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
first part of problem set 4
</commit_message>
<xml_diff>
--- a/time logging.xlsx
+++ b/time logging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steff\Personal\CS Education\Python Introduction course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E339ECF-777B-448F-81B0-FCE4D8735A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4396506F-38D7-4618-B5EA-AF9DBA0B4362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>CS Introduction Lecture 18</t>
+  </si>
+  <si>
+    <t>Problem Set 4</t>
   </si>
 </sst>
 </file>
@@ -473,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE79405-D1A3-4A66-A83E-48D5F1755AB2}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -953,6 +956,46 @@
         <v>22</v>
       </c>
     </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="1">
+        <v>45822</v>
+      </c>
+      <c r="B25">
+        <v>21</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>22</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="1">
+        <v>45823</v>
+      </c>
+      <c r="B26">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>40</v>
+      </c>
+      <c r="D26">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
+      <c r="F26" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
lecture 20 part 1
</commit_message>
<xml_diff>
--- a/time logging.xlsx
+++ b/time logging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffen\Arbejde\CS education\Introduction To CS and Programming Using Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38F2235-C7C3-4922-A716-282703686B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BBAA14-0078-4436-9BF7-A65F7B7A50CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>Problem Set 4</t>
+  </si>
+  <si>
+    <t>CS Introduction Lecture 19</t>
+  </si>
+  <si>
+    <t>CS Introduction Lecture 20</t>
   </si>
 </sst>
 </file>
@@ -476,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE79405-D1A3-4A66-A83E-48D5F1755AB2}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1016,6 +1022,46 @@
         <v>23</v>
       </c>
     </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>45822</v>
+      </c>
+      <c r="B28">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <v>30</v>
+      </c>
+      <c r="D28">
+        <v>16</v>
+      </c>
+      <c r="E28">
+        <v>40</v>
+      </c>
+      <c r="F28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>45824</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>35</v>
+      </c>
+      <c r="D29">
+        <v>21</v>
+      </c>
+      <c r="E29">
+        <v>33</v>
+      </c>
+      <c r="F29" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finger exercise lecture 20
</commit_message>
<xml_diff>
--- a/time logging.xlsx
+++ b/time logging.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffen\Arbejde\CS education\Introduction To CS and Programming Using Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BBAA14-0078-4436-9BF7-A65F7B7A50CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881FF5E7-8E8A-451D-B571-2E3595222CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
+    <workbookView xWindow="38280" yWindow="-1980" windowWidth="16440" windowHeight="28440" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -482,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE79405-D1A3-4A66-A83E-48D5F1755AB2}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1062,6 +1062,26 @@
         <v>25</v>
       </c>
     </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>45825</v>
+      </c>
+      <c r="B30">
+        <v>19</v>
+      </c>
+      <c r="C30">
+        <v>23</v>
+      </c>
+      <c r="D30">
+        <v>20</v>
+      </c>
+      <c r="E30">
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
lecture 20 & 21
</commit_message>
<xml_diff>
--- a/time logging.xlsx
+++ b/time logging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffen\Arbejde\CS education\Introduction To CS and Programming Using Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881FF5E7-8E8A-451D-B571-2E3595222CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A749593A-18F0-4134-9CE0-582FE143039F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-1980" windowWidth="16440" windowHeight="28440" xr2:uid="{A6E14872-8F24-4185-8E44-B3E9C0784B59}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>CS Introduction Lecture 20</t>
+  </si>
+  <si>
+    <t>CS Introduction Lecture 21</t>
+  </si>
+  <si>
+    <t>CS Introduction Lecture 22</t>
   </si>
 </sst>
 </file>
@@ -482,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE79405-D1A3-4A66-A83E-48D5F1755AB2}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1082,6 +1088,46 @@
         <v>25</v>
       </c>
     </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>45826</v>
+      </c>
+      <c r="B31">
+        <v>18</v>
+      </c>
+      <c r="C31">
+        <v>20</v>
+      </c>
+      <c r="D31">
+        <v>18</v>
+      </c>
+      <c r="E31">
+        <v>50</v>
+      </c>
+      <c r="F31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>45826</v>
+      </c>
+      <c r="B32">
+        <v>19</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>20</v>
+      </c>
+      <c r="E32">
+        <v>23</v>
+      </c>
+      <c r="F32" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>